<commit_message>
fixing issues with normalizing by normalized IS
</commit_message>
<xml_diff>
--- a/IOP1_timeline/Sensitivity_analysis_matchparams.xlsx
+++ b/IOP1_timeline/Sensitivity_analysis_matchparams.xlsx
@@ -21,6 +21,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Match_factor_floor</t>
+  </si>
+  <si>
+    <t>Reverse_match_factor_floor</t>
+  </si>
+  <si>
+    <t>LRI_diff_floor</t>
+  </si>
+  <si>
+    <t>mean_pct_volfound</t>
+  </si>
+  <si>
+    <t>median_pct_found</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +356,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>600</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>65.5</v>
+      </c>
+      <c r="E2">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>625</v>
+      </c>
+      <c r="B3">
+        <f>B2</f>
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <f>C2</f>
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>64.72</v>
+      </c>
+      <c r="E3">
+        <v>70.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f>A3+25</f>
+        <v>650</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B11" si="0">B3</f>
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C11" si="1">C3</f>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>63.7</v>
+      </c>
+      <c r="E4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" ref="A5:A11" si="2">A4+25</f>
+        <v>675</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>62.3</v>
+      </c>
+      <c r="E5">
+        <v>67.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>700</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>60.6</v>
+      </c>
+      <c r="E6">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>725</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>750</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>55.9</v>
+      </c>
+      <c r="E8">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>775</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f>A9+25</f>
+        <v>800</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>48.959000000000003</v>
+      </c>
+      <c r="E10">
+        <v>52.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>825</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>750</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>48.6</v>
+      </c>
+      <c r="E12">
+        <v>52.54</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>